<commit_message>
STL map does not release small chunks of memory after map.clear()--glibc malloc/free behavior.
</commit_message>
<xml_diff>
--- a/c_cpp/0001/malloc_bins.xlsx
+++ b/c_cpp/0001/malloc_bins.xlsx
@@ -36,7 +36,7 @@
     <t>unsorted</t>
   </si>
   <si>
-    <t>mmap的阈值</t>
+    <t>mmap分配阈值</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+      <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>